<commit_message>
Homework 2 first commit
</commit_message>
<xml_diff>
--- a/QF620_Stochastic Modelling_in_Finance/Assignment_1/QF620 - Assignment 1.xlsx
+++ b/QF620_Stochastic Modelling_in_Finance/Assignment_1/QF620 - Assignment 1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8da164fcd98d51a/01 Documents/SMU/QF620 Stochastic Modelling in Finance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju/Projects/00_SMU/mqf_practice/QF620_Stochastic Modelling_in_Finance/Assignment_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{2AF14961-CD65-3448-9553-ECCFC2E42DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14C4975C-B4ED-BC44-811A-2A2F365B2D98}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3318029C-9FD3-8944-92E0-DA66DFA88C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="22360" windowWidth="30240" windowHeight="18880" xr2:uid="{0AC1C2CA-FA76-2048-95E9-C6A5A0E09CF6}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="36000" windowHeight="21100" xr2:uid="{0AC1C2CA-FA76-2048-95E9-C6A5A0E09CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -139,10 +139,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -481,7 +482,7 @@
   <dimension ref="B1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,7 +673,7 @@
         <f>MAX($C$6-I8,0)</f>
         <v>5</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3">
         <f>1/(1+$C$5)*($C$7*O7+$C$8*O11)</f>
         <v>1.1982248520710059</v>
       </c>
@@ -898,7 +899,7 @@
         <f>MAX($C$6-I22,0)</f>
         <v>5</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="3">
         <f>MAX(1/(1+$C$5)*($C$7*O21+$C$8*O25),M22-$C$6)</f>
         <v>1.1982248520710059</v>
       </c>

</xml_diff>